<commit_message>
removed euro from data
</commit_message>
<xml_diff>
--- a/data/constraints.xlsx
+++ b/data/constraints.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58527391419e295a/Desktop/04 UW Spring Course/Time Series ^0 Panel Data/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC104864395E6DD25BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A455D6-703F-4B95-A81A-C3EDF3F96E6E}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_F25DC773A252ABDACC104864395E6DD25BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C39F7913-7592-45A3-A258-77B9DAD5A1FA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country-code" sheetId="1" r:id="rId1"/>
-    <sheet name="time-period" sheetId="2" r:id="rId2"/>
+    <sheet name="dropped-country-codes" sheetId="3" r:id="rId2"/>
+    <sheet name="time-period" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
   <si>
     <t>iso_a3</t>
   </si>
@@ -107,15 +108,6 @@
   </si>
   <si>
     <t>Denmark</t>
-  </si>
-  <si>
-    <t>EUZ</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>Euro area</t>
   </si>
   <si>
     <t>HKG</t>
@@ -589,9 +581,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -701,200 +695,134 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -903,16 +831,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4038FA72-7887-48E1-B1B7-A6EF3E640F85}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1AFCA4-387F-4DEE-9C16-C0E80FF2CA74}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>